<commit_message>
fix typo of humdity instead of humidity
</commit_message>
<xml_diff>
--- a/data/song/collated/HSPi-Round-1-Heat-Trials.xlsx
+++ b/data/song/collated/HSPi-Round-1-Heat-Trials.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$Y$999</definedName>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">temp_median</t>
   </si>
   <si>
-    <t xml:space="preserve">humdity_mean</t>
+    <t xml:space="preserve">humidity_mean</t>
   </si>
   <si>
     <t xml:space="preserve">T229</t>
@@ -223,15 +223,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF101010"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -243,6 +243,112 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -251,7 +357,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>